<commit_message>
add charts to show expenditure and balance dist
</commit_message>
<xml_diff>
--- a/finance-manager/wallet-manager.xlsx
+++ b/finance-manager/wallet-manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github-rebuild\excel-works\finance-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AC360D-BCDB-458C-8C37-2466DEE95F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE3769E-922A-41A5-A870-57F7958DC404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="238">
   <si>
     <t>Wallet App Root</t>
   </si>
@@ -728,6 +728,24 @@
   </si>
   <si>
     <t>Starting Balance</t>
+  </si>
+  <si>
+    <t>Mobile Recharge</t>
+  </si>
+  <si>
+    <t>Grameenphone</t>
+  </si>
+  <si>
+    <t>bKash Recharge - Rakib</t>
+  </si>
+  <si>
+    <t>Telecom</t>
+  </si>
+  <si>
+    <t>Gift</t>
+  </si>
+  <si>
+    <t>Gift - Sifat</t>
   </si>
   <si>
     <t>xxxx xxxx xxxx xxxx</t>
@@ -852,7 +870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -874,7 +892,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -892,6 +909,1768 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Payment Medium</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Summary</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Dashboard-Oct22'!$F$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Amount</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F76A-430D-9B17-2636FE24D675}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-F76A-430D-9B17-2636FE24D675}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-A590-44A8-ACC0-076A2F2DEA56}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Dashboard-Oct22'!$E$8:$E$10</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Bank</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>E-wallet</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Cash</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dashboard-Oct22'!$F$8:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>_([$BDT]\ * #,##0.00_);_([$BDT]\ * \(#,##0.00\);_([$BDT]\ * "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>609</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A590-44A8-ACC0-076A2F2DEA56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="60"/>
+      </c:doughnutChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Current Balance Distribution</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Dashboard-Oct22'!$I$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Amount</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Dashboard-Oct22'!$H$8:$H$10</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Bank</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>E-wallet</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Cash</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dashboard-Oct22'!$I$8:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>_([$BDT]\ * #,##0.00_);_([$BDT]\ * \(#,##0.00\);_([$BDT]\ * "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>61068.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1830.2600000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10759</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-879C-45DC-9F08-4151EB8C2350}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1854568927"/>
+        <c:axId val="1854591807"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1854568927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1854591807"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1854591807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$BDT]\ * #,##0.00_);_([$BDT]\ * \(#,##0.00\);_([$BDT]\ * &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1854568927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>847725</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50BE0646-1444-CBFB-9188-33316979427E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4692FABC-282B-D712-DF8E-CBD8F58B87FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1160,7 +2939,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1229,7 +3008,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="F6" s="5">
         <v>153.25</v>
@@ -1256,7 +3035,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="F7" s="5">
         <v>439.26</v>
@@ -1283,7 +3062,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="F8" s="5">
         <v>0</v>
@@ -1401,7 +3180,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1449,7 +3228,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="I4" s="5"/>
     </row>
@@ -1464,7 +3243,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="I5" s="5"/>
     </row>
@@ -1479,7 +3258,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="I6" s="5"/>
     </row>
@@ -1679,9 +3458,12 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99B2AAA8-DC2F-4F97-9467-6B761BFB1C2D}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="B1:N73"/>
+  <dimension ref="B1:N75"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1689,10 +3471,10 @@
     <col min="2" max="2" width="20.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="16" style="2" customWidth="1"/>
     <col min="4" max="4" width="42.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" style="2" customWidth="1"/>
-    <col min="8" max="11" width="15.7109375" style="2" customWidth="1"/>
+    <col min="8" max="11" width="15.7109375" style="5" customWidth="1"/>
     <col min="12" max="12" width="14.7109375" style="2" customWidth="1"/>
     <col min="13" max="13" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.85546875" style="2" bestFit="1" customWidth="1"/>
@@ -1703,16 +3485,24 @@
       <c r="B1" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="E1" s="2"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="3" spans="2:14" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="2"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="5" spans="2:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
@@ -1724,7 +3514,7 @@
       <c r="D5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="12" t="s">
@@ -1733,16 +3523,16 @@
       <c r="G5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="5" t="s">
         <v>27</v>
       </c>
       <c r="L5" s="12" t="s">
@@ -3115,14 +4905,14 @@
         <v>60</v>
       </c>
       <c r="I38" s="5">
-        <f t="shared" ref="I38:I73" si="2">$E38*$H38</f>
+        <f t="shared" ref="I38:I75" si="2">$E38*$H38</f>
         <v>60</v>
       </c>
       <c r="J38" s="5">
         <v>0</v>
       </c>
       <c r="K38" s="5">
-        <f t="shared" ref="K38:K73" si="3">$I38-$J38</f>
+        <f t="shared" ref="K38:K75" si="3">$I38-$J38</f>
         <v>60</v>
       </c>
       <c r="L38" s="2" t="s">
@@ -4511,6 +6301,86 @@
         <v>44836</v>
       </c>
       <c r="N73" s="5"/>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B74" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E74" s="2">
+        <v>1</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H74" s="5">
+        <v>109</v>
+      </c>
+      <c r="I74" s="5">
+        <f t="shared" si="2"/>
+        <v>109</v>
+      </c>
+      <c r="J74" s="5">
+        <v>0</v>
+      </c>
+      <c r="K74" s="5">
+        <f t="shared" si="3"/>
+        <v>109</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M74" s="17">
+        <v>44837</v>
+      </c>
+      <c r="N74" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B75" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E75" s="2">
+        <v>1</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H75" s="5">
+        <v>500</v>
+      </c>
+      <c r="I75" s="5">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="J75" s="5">
+        <v>0</v>
+      </c>
+      <c r="K75" s="5">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M75" s="17">
+        <v>44837</v>
+      </c>
+      <c r="N75" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4543,11 +6413,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="2:9" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>215</v>
       </c>
     </row>
@@ -4619,14 +6489,14 @@
       </c>
       <c r="F9" s="5">
         <f>SUMIF('Transactions-Oct22'!$L:$L,Base!$L7,'Transactions-Oct22'!$K:$K)</f>
-        <v>0</v>
+        <v>609</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>166</v>
       </c>
       <c r="I9" s="5">
         <f>$C13+SUMIFS(Transfers!$F:$F,Transfers!$E:$E,Base!$L7,Transfers!$I:$I,MONTH('Dashboard-Oct22'!$C$3),Transfers!$J:$J,YEAR('Dashboard-Oct22'!$C$3))-SUMIFS(Transfers!$F:$F,Transfers!$C:$C,Base!$L7,Transfers!$I:$I,MONTH('Dashboard-Oct22'!$C$3),Transfers!$J:$J,YEAR('Dashboard-Oct22'!$C$3))-SUMIFS('Transactions-Oct22'!$K:$K,'Transactions-Oct22'!$L:$L,Base!$L7)</f>
-        <v>2439.2600000000002</v>
+        <v>1830.2600000000002</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -4665,14 +6535,14 @@
       </c>
       <c r="F11" s="11">
         <f>SUM($F$8:$F$10)</f>
-        <v>15995</v>
+        <v>16604</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>223</v>
       </c>
       <c r="I11" s="11">
         <f>SUM($I$8:$I$10)</f>
-        <v>74266.510000000009</v>
+        <v>73657.510000000009</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
@@ -4713,5 +6583,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>